<commit_message>
adds thrust to UI. program now reads dat files when dropped in
</commit_message>
<xml_diff>
--- a/data/AT5330KV220.xlsx
+++ b/data/AT5330KV220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc5b649c178b8907/Desktop/clubs/Ground-Roll-Calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC104876599E52165BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AC58987-9088-46FE-8EF5-AFF5B6E5EFB5}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC104876599E52165BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E67D521C-C441-47BC-8E6E-44654607F461}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,13 +36,13 @@
     <t>Propeller</t>
   </si>
   <si>
-    <t>18*10</t>
+    <t>18x10</t>
   </si>
   <si>
-    <t>19*10</t>
+    <t>19x10</t>
   </si>
   <si>
-    <t>20*10</t>
+    <t>20x10</t>
   </si>
 </sst>
 </file>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>